<commit_message>
Esboço do BD atualizado
</commit_message>
<xml_diff>
--- a/esboço_BD.xlsx
+++ b/esboço_BD.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitor.herculano\OneDrive - Accenture\Documents\Bandtec\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitor.herculano\OneDrive - Accenture\Documents\Bandtec\SegundoSemestre\Bandtec_TotemHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDB58A8E-DBB8-45B8-BA55-9F0468C1A1E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55115CD-66E0-4742-87C3-76560E3D3AF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F31420F3-A342-4F5A-AD70-4AD509DAF3CB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{F31420F3-A342-4F5A-AD70-4AD509DAF3CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="77">
   <si>
     <t>Id_Cliente</t>
   </si>
@@ -169,14 +170,118 @@
   </si>
   <si>
     <t>Recebido Wifi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cliente </t>
+  </si>
+  <si>
+    <t>id_cliente</t>
+  </si>
+  <si>
+    <t>nome_cliente</t>
+  </si>
+  <si>
+    <t>cnpj_cliente</t>
+  </si>
+  <si>
+    <t>senha_cliente</t>
+  </si>
+  <si>
+    <t>Um cliente(linha) tem várias estações</t>
+  </si>
+  <si>
+    <t>Linha</t>
+  </si>
+  <si>
+    <t>Estações</t>
+  </si>
+  <si>
+    <t>ID_ESTAÇÃO</t>
+  </si>
+  <si>
+    <t>nome_estação</t>
+  </si>
+  <si>
+    <t>fk_linha</t>
+  </si>
+  <si>
+    <t>qtd_estações</t>
+  </si>
+  <si>
+    <t>Uma estação possui de  1 a 4 Totens</t>
+  </si>
+  <si>
+    <t>Totens</t>
+  </si>
+  <si>
+    <t>id_totem</t>
+  </si>
+  <si>
+    <t>fk_estação</t>
+  </si>
+  <si>
+    <t>id_user</t>
+  </si>
+  <si>
+    <t>fk_cliente</t>
+  </si>
+  <si>
+    <t>estação</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>senha</t>
+  </si>
+  <si>
+    <t>Usuários do Sistema</t>
+  </si>
+  <si>
+    <t>Um cliente pode ter 1 ou mais usuários</t>
+  </si>
+  <si>
+    <t>fk_user</t>
+  </si>
+  <si>
+    <t>1:n</t>
+  </si>
+  <si>
+    <t>Uma estação pode ter 1 ou mais usuários</t>
+  </si>
+  <si>
+    <t>Totem_ativo</t>
+  </si>
+  <si>
+    <t>CPU % utilizada</t>
+  </si>
+  <si>
+    <t>CPU_SPEED</t>
+  </si>
+  <si>
+    <t>Memoria consumida</t>
+  </si>
+  <si>
+    <t>%disk_utlizada</t>
+  </si>
+  <si>
+    <t>GPU %utilizada</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -192,7 +297,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -252,11 +357,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -264,16 +393,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -287,6 +407,50 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,6 +680,311 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>527050</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Arrow: Down 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A748D3D-F5A7-4C51-A9F7-9E4391714929}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="990600" y="1631950"/>
+          <a:ext cx="146050" cy="495300"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>155575</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>320675</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Arrow: Down 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98AA7E56-34CD-418C-9C4A-49105FF1D36A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="2768600" y="374650"/>
+          <a:ext cx="146050" cy="495300"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>85487</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>70672</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>254426</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>283216</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Arrow: Down 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{004D3032-2EA7-4FF3-BADF-9706C3F9392B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="13468699">
+          <a:off x="4759087" y="1766122"/>
+          <a:ext cx="168939" cy="1165044"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>321595</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>91246</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>210522</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>78278</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Arrow: Down 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDC6D52E-BD2E-40AE-8574-0CC9F1BED1C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16871240">
+          <a:off x="2310893" y="2978748"/>
+          <a:ext cx="177532" cy="498527"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>200944</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>72197</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>489921</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>65579</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Arrow: Down 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EA0D1E1-FEFF-40CC-823C-0B7863FF8FDC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="6533642" y="279999"/>
+          <a:ext cx="177532" cy="498527"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -820,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A0A754B-C39F-4CE2-842D-6F77171DFA7B}">
   <dimension ref="B2:K25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView showGridLines="0" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16:J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -835,109 +1304,109 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="K11" s="6"/>
+      <c r="K11" s="10"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="F12" s="3" t="s">
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="F12" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -945,17 +1414,17 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="J13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -963,131 +1432,131 @@
       <c r="D14" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G14" s="1"/>
-      <c r="J14" s="3" t="s">
+      <c r="J14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="J15" s="3" t="s">
+      <c r="J15" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="J16" s="3" t="s">
+      <c r="J16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="J17" s="3" t="s">
+      <c r="J17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="J18" s="3" t="s">
+      <c r="J18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="J19" s="3" t="s">
+      <c r="J19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K19" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="J20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="K20" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="J21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="K21" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="J22" s="3" t="s">
+      <c r="J22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="K22" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="J23" s="3" t="s">
+      <c r="J23" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="K23" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="J24" s="3" t="s">
+      <c r="J24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K24" s="4" t="s">
+      <c r="K24" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="J25" s="10" t="s">
+      <c r="J25" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K25" s="11" t="s">
+      <c r="K25" s="8" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1106,4 +1575,235 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F4CF4B-3446-426F-9F14-227DA0BD6564}">
+  <dimension ref="B4:O19"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="4.7265625" customWidth="1"/>
+    <col min="6" max="6" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" customWidth="1"/>
+    <col min="8" max="8" width="4" customWidth="1"/>
+    <col min="11" max="11" width="3" customWidth="1"/>
+    <col min="14" max="14" width="4" customWidth="1"/>
+    <col min="15" max="15" width="23.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C5" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="I5" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="13"/>
+      <c r="O5" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C6" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="F6" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="I6" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="14"/>
+      <c r="L6" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="M6" s="17"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C7" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="I7" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" s="14"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="M7" s="16"/>
+      <c r="O7" s="20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C8" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="I8" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8" s="14"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="O8" s="20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C9" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="I9" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="14"/>
+      <c r="O9" s="20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C10" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="O10" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C11" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="O11" s="20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="O12" s="20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C13" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="22"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="O13" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="F14" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="J14" s="12"/>
+      <c r="O14" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="F15" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="O15" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F16" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="O16" s="20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="6:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F17" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="O17" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="6:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F18" s="25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="6:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F19" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="L7:M8"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="C13:D15"/>
+    <mergeCell ref="I14:J15"/>
+    <mergeCell ref="H12:I13"/>
+    <mergeCell ref="F7:G8"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>